<commit_message>
Fixed bugs in Uploader, GUI; Modified and polished JSON creation.
</commit_message>
<xml_diff>
--- a/src/test/resources/Test 1.xlsx
+++ b/src/test/resources/Test 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesle\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesle\Documents\School\C01\Team17\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF577F11-B6A8-4670-8C54-8CB284268D97}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DA19C8-F08A-48EB-8AFD-59ADBE671FBF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9144" xr2:uid="{DE75E0F5-C35D-46DA-9B7C-F2DEBD0E6A1E}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>AB</t>
   </si>
@@ -60,6 +60,9 @@
 iCARE - Immigration Contribution Agreement Reporting Environment
 Information and Orientation
 </t>
+  </si>
+  <si>
+    <t>children</t>
   </si>
 </sst>
 </file>
@@ -67,10 +70,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -132,10 +135,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -466,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38AC212C-6C07-438A-AA17-E1D25A9C4160}">
-  <dimension ref="A1:CQ5"/>
+  <dimension ref="A1:CQ8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,6 +603,9 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:95" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -613,6 +619,9 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:95" x14ac:dyDescent="0.3">
@@ -627,6 +636,24 @@
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding changes required to implement the early stages of the conflict resolver
</commit_message>
<xml_diff>
--- a/src/test/resources/Test 1.xlsx
+++ b/src/test/resources/Test 1.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesle\Documents\School\C01\Team17\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radulaudat/Desktop/Team17/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DA19C8-F08A-48EB-8AFD-59ADBE671FBF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9144" xr2:uid="{DE75E0F5-C35D-46DA-9B7C-F2DEBD0E6A1E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -50,12 +55,6 @@
     <t>alice</t>
   </si>
   <si>
-    <t>employment</t>
-  </si>
-  <si>
-    <t>housing</t>
-  </si>
-  <si>
     <t xml:space="preserve">Immigration, Refugees and Citizenship Canada
 iCARE - Immigration Contribution Agreement Reporting Environment
 Information and Orientation
@@ -64,16 +63,22 @@
   <si>
     <t>children</t>
   </si>
+  <si>
+    <t xml:space="preserve">employment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  housing  </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -135,10 +140,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -151,13 +156,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Comma [0] 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Comma 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Currency [0] 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Currency 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Comma [0] 2" xfId="6"/>
+    <cellStyle name="Comma 2" xfId="5"/>
+    <cellStyle name="Currency [0] 2" xfId="4"/>
+    <cellStyle name="Currency 2" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Percent 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Percent 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -468,18 +473,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38AC212C-6C07-438A-AA17-E1D25A9C4160}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CQ8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:95" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:95" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -576,7 +581,7 @@
       <c r="CP1" s="3"/>
       <c r="CQ1" s="3"/>
     </row>
-    <row r="2" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -590,7 +595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -604,10 +609,10 @@
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:95" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -618,13 +623,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -635,23 +640,23 @@
         <v>1.8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:95" x14ac:dyDescent="0.2">
       <c r="E6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:95" x14ac:dyDescent="0.2">
       <c r="E7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:95" x14ac:dyDescent="0.2">
       <c r="E8">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Revert "adding changes required to implement the early stages of the conflict…"
</commit_message>
<xml_diff>
--- a/src/test/resources/Test 1.xlsx
+++ b/src/test/resources/Test 1.xlsx
@@ -1,28 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radulaudat/Desktop/Team17/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesle\Documents\School\C01\Team17\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DA19C8-F08A-48EB-8AFD-59ADBE671FBF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9144" xr2:uid="{DE75E0F5-C35D-46DA-9B7C-F2DEBD0E6A1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -55,6 +50,12 @@
     <t>alice</t>
   </si>
   <si>
+    <t>employment</t>
+  </si>
+  <si>
+    <t>housing</t>
+  </si>
+  <si>
     <t xml:space="preserve">Immigration, Refugees and Citizenship Canada
 iCARE - Immigration Contribution Agreement Reporting Environment
 Information and Orientation
@@ -63,22 +64,16 @@
   <si>
     <t>children</t>
   </si>
-  <si>
-    <t xml:space="preserve">employment </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  housing  </t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -140,10 +135,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -156,13 +151,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Comma [0] 2" xfId="6"/>
-    <cellStyle name="Comma 2" xfId="5"/>
-    <cellStyle name="Currency [0] 2" xfId="4"/>
-    <cellStyle name="Currency 2" xfId="3"/>
+    <cellStyle name="Comma [0] 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Currency [0] 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Currency 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Percent 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Percent 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -473,18 +468,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38AC212C-6C07-438A-AA17-E1D25A9C4160}">
   <dimension ref="A1:CQ8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:95" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:95" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -581,7 +576,7 @@
       <c r="CP1" s="3"/>
       <c r="CQ1" s="3"/>
     </row>
-    <row r="2" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:95" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -595,7 +590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:95" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -609,10 +604,10 @@
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:95" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:95" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -623,13 +618,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:95" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -640,23 +635,23 @@
         <v>1.8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:95" x14ac:dyDescent="0.3">
       <c r="E6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:95" x14ac:dyDescent="0.3">
       <c r="E7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:95" x14ac:dyDescent="0.3">
       <c r="E8">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
adding files with corrections as pointed out during merge request, as well as tests
</commit_message>
<xml_diff>
--- a/src/test/resources/Test 1.xlsx
+++ b/src/test/resources/Test 1.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>AB</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t xml:space="preserve">  housing  </t>
+  </si>
+  <si>
+    <t>mistakes</t>
+  </si>
+  <si>
+    <t>first mistake</t>
   </si>
 </sst>
 </file>
@@ -477,7 +483,7 @@
   <dimension ref="A1:CQ8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -647,6 +653,18 @@
       </c>
     </row>
     <row r="6" spans="1:95" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="E6">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
adding some test file
</commit_message>
<xml_diff>
--- a/src/test/resources/Test 1.xlsx
+++ b/src/test/resources/Test 1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesle\Documents\SCHOOL\C01\Team17\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radulaudat/Desktop/Team17/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF71875-F283-4EEE-88D5-2A5F4393A9EA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="23040" windowHeight="9135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7420" yWindow="1040" windowWidth="23040" windowHeight="9140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,11 +19,11 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -72,12 +71,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -139,10 +138,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -155,13 +154,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Comma [0] 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Comma 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Currency [0] 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Currency 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Comma [0] 2" xfId="6"/>
+    <cellStyle name="Comma 2" xfId="5"/>
+    <cellStyle name="Currency [0] 2" xfId="4"/>
+    <cellStyle name="Currency 2" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Percent 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Percent 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -472,16 +471,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CQ9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:95" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:95" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -580,7 +579,7 @@
       <c r="CP1" s="3"/>
       <c r="CQ1" s="3"/>
     </row>
-    <row r="2" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -594,7 +593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -611,7 +610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -628,7 +627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -645,7 +644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -653,7 +652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -661,7 +660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -669,7 +668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>

</xml_diff>